<commit_message>
Updated BOM for SMT
</commit_message>
<xml_diff>
--- a/Components/Jacdac_3D_Magnetometer_BOM.xlsx
+++ b/Components/Jacdac_3D_Magnetometer_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\Jacdac\Jacdac-3D-Magnetometer\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C1771C-B97F-41AD-821B-7F6F177E2A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA157A3-AE1C-4041-899C-FF1956301AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RevA" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="156">
   <si>
     <t>Index</t>
   </si>
@@ -319,18 +319,9 @@
     <t>https://lcsc.com/product-detail/ST-Microelectronics_STMicroelectronics-STM32G030F6P6_C724040.html</t>
   </si>
   <si>
-    <t>C3015484</t>
-  </si>
-  <si>
     <t>XC6206-3.3V</t>
   </si>
   <si>
-    <t>IC REG LINEAR 3.3V SOT-23</t>
-  </si>
-  <si>
-    <t>https://lcsc.com/product-detail/Linear-Voltage-Regulators-LDO_YONGYUTAI-XC6206-3-3V_C3015484.html</t>
-  </si>
-  <si>
     <t>470R</t>
   </si>
   <si>
@@ -373,21 +364,6 @@
     <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Viking-Tech-AR02BTC1500_C319855.html</t>
   </si>
   <si>
-    <t>CRCW0402220RFKED</t>
-  </si>
-  <si>
-    <t>C482103</t>
-  </si>
-  <si>
-    <t>RES 220 OHM 1% 0402</t>
-  </si>
-  <si>
-    <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Vishay-Intertech-CRCW0402220RFKED_C482103.html</t>
-  </si>
-  <si>
-    <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Viking-Tech-AR02BTC4701_C317921.html</t>
-  </si>
-  <si>
     <t>IC2</t>
   </si>
   <si>
@@ -466,9 +442,6 @@
     <t>R3,R5</t>
   </si>
   <si>
-    <t>LED (D1)</t>
-  </si>
-  <si>
     <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Viking-Tech-ARG02BTC1002_C2902636.html</t>
   </si>
   <si>
@@ -482,6 +455,51 @@
   </si>
   <si>
     <t>C2902636</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>https://www.arrow.com/en/products/tlv493da1b6htsa2/infineon-technologies-ag?q=TLV493DA1B6HTSA2</t>
+  </si>
+  <si>
+    <t>TLV493DA1B6HTSA2/C126688</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_TDK-C1005X5R1A475KTJ00E_C342983.html</t>
+  </si>
+  <si>
+    <t>BAT54S</t>
+  </si>
+  <si>
+    <t>C328578</t>
+  </si>
+  <si>
+    <t>BAT54S,23</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Schottky-Barrier-Diodes-SBD_Foshan-Blue-Rocket-Elec-BAT54S_C328578.html</t>
+  </si>
+  <si>
+    <t>C317911</t>
+  </si>
+  <si>
+    <t>AR02BTC2200</t>
+  </si>
+  <si>
+    <t>RES 220 OHM 0.1% 0402</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Viking-Tech-AR02BTC2200_C317911.html</t>
+  </si>
+  <si>
+    <t>C2891841</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V  SOT-23-3L</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Linear-Voltage-Regulators-LDO_YONGYUTAI-XC6206-3-3V_C2891841.html</t>
   </si>
 </sst>
 </file>
@@ -1381,23 +1399,23 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" customWidth="1"/>
+    <col min="6" max="6" width="25.54296875" customWidth="1"/>
+    <col min="7" max="7" width="32.81640625" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="77.85546875" customWidth="1"/>
+    <col min="10" max="10" width="77.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1429,7 +1447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1462,7 +1480,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1495,7 +1513,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1528,7 +1546,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1561,7 +1579,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1594,7 +1612,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1627,7 +1645,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1663,7 +1681,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1696,7 +1714,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1729,7 +1747,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1762,7 +1780,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1795,7 +1813,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1828,7 +1846,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1861,7 +1879,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1896,7 +1914,7 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.75">
       <c r="H18" s="4" t="s">
         <v>7</v>
       </c>
@@ -1932,23 +1950,23 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" customWidth="1"/>
+    <col min="6" max="6" width="25.54296875" customWidth="1"/>
+    <col min="7" max="7" width="32.81640625" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="77.85546875" customWidth="1"/>
+    <col min="10" max="10" width="77.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1980,9 +1998,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -1991,16 +2009,16 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="H2" s="1">
         <v>2.3300000000000001E-2</v>
@@ -2010,63 +2028,63 @@
         <v>4.6600000000000003E-2</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="H3" s="1">
-        <v>4.0899999999999999E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="I3" s="1">
         <f>H3*B3</f>
-        <v>4.0899999999999999E-2</v>
+        <v>5.4399999999999997E-2</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H4" s="1">
         <v>3.9399999999999998E-2</v>
@@ -2076,57 +2094,57 @@
         <v>3.9399999999999998E-2</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H5" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I8" si="0">H5*B5</f>
+        <f t="shared" ref="I5" si="0">H5*B5</f>
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>48</v>
@@ -2142,21 +2160,21 @@
         <v>3.27</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>51</v>
@@ -2181,9 +2199,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -2192,95 +2210,95 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="H8" s="1">
-        <v>4.0800000000000003E-2</v>
+        <v>6.1400000000000003E-2</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="0"/>
-        <v>4.0800000000000003E-2</v>
+        <f t="shared" ref="I8" si="1">H8*B8</f>
+        <v>6.1400000000000003E-2</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="H9" s="1">
         <v>2.2700000000000001E-2</v>
       </c>
       <c r="I9" s="1">
         <f>H9*B9</f>
-        <v>2.2700000000000001E-2</v>
+        <v>4.5400000000000003E-2</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="H10" s="1">
         <v>4.7600000000000003E-2</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" ref="I10:I11" si="1">H10*B10</f>
-        <v>0.14280000000000001</v>
+        <f t="shared" ref="I10:I12" si="2">H10*B10</f>
+        <v>9.5200000000000007E-2</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2288,34 +2306,34 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H11" s="1">
         <v>3.3500000000000002E-2</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3500000000000002E-2</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -2324,49 +2342,49 @@
         <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H12" s="1">
         <v>3.0800000000000001E-2</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" ref="I12" si="2">H12*B12</f>
+        <f t="shared" si="2"/>
         <v>3.0800000000000001E-2</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H13" s="1">
         <v>2.8899999999999999E-2</v>
@@ -2376,68 +2394,68 @@
         <v>2.8899999999999999E-2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A14" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>145</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="1">
-        <v>0.03</v>
+        <v>2.4500000000000001E-2</v>
       </c>
       <c r="I14" s="1">
         <f>H14*B14</f>
-        <v>0.03</v>
+        <v>2.4500000000000001E-2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.75">
       <c r="H17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I17" s="1">
         <f>SUM(I2:I14)</f>
-        <v>4.7384000000000013</v>
+        <v>4.7420999999999998</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K6" r:id="rId1" xr:uid="{5F5BE1C5-E780-43CD-A79E-3431C36D8A75}"/>
-    <hyperlink ref="J5" r:id="rId2" xr:uid="{B77F362C-F389-48B4-B69E-814CC8C3C6A5}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{63BD6AA9-05E1-47DB-829F-51E06E974AF5}"/>
-    <hyperlink ref="J14" r:id="rId4" xr:uid="{970A0BF8-84C4-4080-9C8C-2605A5CADABD}"/>
-    <hyperlink ref="J12" r:id="rId5" xr:uid="{11A59C22-5B1A-423C-A11C-64FC560D83AD}"/>
-    <hyperlink ref="J13" r:id="rId6" xr:uid="{AA4E1286-4915-496B-B5A7-5C42DDE36BA3}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{E628435E-0BFB-47FA-86B1-34F41CCC5A46}"/>
-    <hyperlink ref="J7" r:id="rId8" xr:uid="{A99B65C7-3937-465D-AC38-C8ADDBF1B86B}"/>
-    <hyperlink ref="J6" r:id="rId9" xr:uid="{9F452534-E4C4-4CE1-A86F-4C2ACC1F396F}"/>
-    <hyperlink ref="J9" r:id="rId10" xr:uid="{DCA8AC2C-7032-42F7-B019-2F5D8684B3FA}"/>
-    <hyperlink ref="J11" r:id="rId11" xr:uid="{5B9D1A35-D884-4750-BB2D-0E2F9C5012E9}"/>
-    <hyperlink ref="J10" r:id="rId12" xr:uid="{2EC7B85B-475E-44CD-970C-F86A181D5E4E}"/>
-    <hyperlink ref="J4" r:id="rId13" xr:uid="{30512338-C18F-4C1B-BA1C-8750803A87FA}"/>
-    <hyperlink ref="J2" r:id="rId14" xr:uid="{E6CC35AA-AB8D-4D7A-8D4B-C91BF1250F9F}"/>
+    <hyperlink ref="K6" r:id="rId1" xr:uid="{C3F6A1E7-17D5-4BD8-B620-4DB566EC6693}"/>
+    <hyperlink ref="J14" r:id="rId2" xr:uid="{2A4601CC-2630-4340-8B3F-BBC3CDC591B3}"/>
+    <hyperlink ref="J12" r:id="rId3" xr:uid="{83F20078-4346-4B10-ABC4-0E1A56F67129}"/>
+    <hyperlink ref="J13" r:id="rId4" xr:uid="{BCB82A1D-6016-4BCB-B051-56B197FB54F1}"/>
+    <hyperlink ref="J7" r:id="rId5" xr:uid="{ADCE8DC4-6ABA-4C51-8E5E-663460578FC0}"/>
+    <hyperlink ref="J6" r:id="rId6" xr:uid="{1923C6FE-FCDF-4FB9-8229-AEB2C733CB31}"/>
+    <hyperlink ref="J9" r:id="rId7" xr:uid="{4B54B73F-B526-4ED4-9F1C-DA8D30D75740}"/>
+    <hyperlink ref="J11" r:id="rId8" xr:uid="{934F2DB3-EF58-45F9-9E3E-8292BCD09FBF}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{7B3307EE-4627-4284-93F8-CE882D51E2E8}"/>
+    <hyperlink ref="J5" r:id="rId10" xr:uid="{8C21FDC5-1B67-4984-9FF5-DC10ACBE6D74}"/>
+    <hyperlink ref="J3" r:id="rId11" xr:uid="{3C0C647D-62D9-4751-85D2-083E8EA409A8}"/>
+    <hyperlink ref="J4" r:id="rId12" xr:uid="{1DC47656-7CA5-420A-9C29-D83141377651}"/>
+    <hyperlink ref="J2" r:id="rId13" xr:uid="{EDFEF2BB-D179-44F3-B37A-01850665B5C9}"/>
+    <hyperlink ref="J8" r:id="rId14" xr:uid="{A387F2B4-EB41-49CD-8548-F2C9E1B5ABDB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>